<commit_message>
Adding evolution of companies meeting criteria over time
</commit_message>
<xml_diff>
--- a/indicators.xlsx
+++ b/indicators.xlsx
@@ -1106,12 +1106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1126,13 +1132,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1415,9 +1424,9 @@
   <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4283,7 +4292,7 @@
       <c r="F110" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G110" s="1" t="s">
+      <c r="G110" s="4" t="s">
         <v>346</v>
       </c>
       <c r="H110" t="s">

</xml_diff>